<commit_message>
Teste de busca com clique
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/HUB_Appium/TestData/BancoDados.xlsx
+++ b/src/main/java/br/com/rsinet/HUB_Appium/TestData/BancoDados.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoAppiumTDD\src\test\java\br\com\rsinet\HUB_Appium\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoAppiumBDD\src\main\java\br\com\rsinet\HUB_Appium\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{AAF97C55-3649-4F4E-879A-460B5D6F4CFC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A767C142-4442-48DC-ABC2-AE31C9DC683B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}" yWindow="-108"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cadastro" r:id="rId1" sheetId="1"/>
-    <sheet name="Pesquisa" r:id="rId2" sheetId="2"/>
+    <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
+    <sheet name="Pesquisa" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Trocar@123</t>
   </si>
@@ -125,18 +125,6 @@
   </si>
   <si>
     <t>Cidade</t>
-  </si>
-  <si>
-    <t>18lPxy</t>
-  </si>
-  <si>
-    <t>sI5pfp</t>
-  </si>
-  <si>
-    <t>U8nj8v</t>
-  </si>
-  <si>
-    <t>imNobL</t>
   </si>
   <si>
     <t>PHrJVq</t>
@@ -146,7 +134,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -220,36 +207,36 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="6" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
       <color rgb="FFFF3300"/>
@@ -271,10 +258,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -309,7 +296,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -361,7 +348,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -472,21 +459,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -503,7 +490,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -555,29 +542,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="2" width="8.88671875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="11.109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="26.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="13.6640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="12.21875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="13.44140625" collapsed="true"/>
-    <col min="7" max="16384" style="2" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="8.88671875" style="2" collapsed="1"/>
+    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.21875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="8.88671875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -606,7 +593,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -656,29 +643,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2" xr:uid="{46AC47A1-1F89-45AF-8C7B-F4A195208066}"/>
-    <hyperlink r:id="rId2" ref="C2" xr:uid="{85BD8E5A-7C04-41EF-BADE-536F55EA589D}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{46AC47A1-1F89-45AF-8C7B-F4A195208066}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{85BD8E5A-7C04-41EF-BADE-536F55EA589D}"/>
   </hyperlinks>
-  <pageMargins bottom="0.78740157499999996" footer="0.31496062000000002" header="0.31496062000000002" left="0.511811024" right="0.511811024" top="0.78740157499999996"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="300"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9334BD-5787-4860-8F04-DE32560FFDB3}">
-  <dimension ref="A1:K15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9334BD-5787-4860-8F04-DE32560FFDB3}">
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.6640625" collapsed="true"/>
-    <col min="3" max="6" style="2" width="8.88671875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="10.88671875" collapsed="true"/>
-    <col min="8" max="16384" style="2" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="6" width="8.88671875" style="2" collapsed="1"/>
+    <col min="7" max="7" width="10.88671875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -756,9 +743,9 @@
         <v>11</v>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="7" spans="1:10" x14ac:dyDescent="0.3"/>
-    <row customHeight="1" ht="13.8" r="8" spans="1:10" x14ac:dyDescent="0.3"/>
-    <row customHeight="1" ht="13.8" r="9" spans="1:10" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="9" t="s">
@@ -797,7 +784,7 @@
       <c r="J15" s="6"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.78740157499999996" footer="0.31496062000000002" header="0.31496062000000002" left="0.511811024" right="0.511811024" top="0.78740157499999996"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Teste concluido com sucesso
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/HUB_Appium/TestData/BancoDados.xlsx
+++ b/src/main/java/br/com/rsinet/HUB_Appium/TestData/BancoDados.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="108">
   <si>
     <t>Trocar@123</t>
   </si>
@@ -140,6 +140,222 @@
   </si>
   <si>
     <t>iANjqP</t>
+  </si>
+  <si>
+    <t>XERkc9</t>
+  </si>
+  <si>
+    <t>HeIILN</t>
+  </si>
+  <si>
+    <t>82Qn7p</t>
+  </si>
+  <si>
+    <t>x908f8</t>
+  </si>
+  <si>
+    <t>k39S3m</t>
+  </si>
+  <si>
+    <t>EpVRdk</t>
+  </si>
+  <si>
+    <t>9RP55N</t>
+  </si>
+  <si>
+    <t>rG8UWW</t>
+  </si>
+  <si>
+    <t>l1ya85</t>
+  </si>
+  <si>
+    <t>47cUsX</t>
+  </si>
+  <si>
+    <t>wtsvie</t>
+  </si>
+  <si>
+    <t>sgytCk</t>
+  </si>
+  <si>
+    <t>6DY5Q1</t>
+  </si>
+  <si>
+    <t>XHfi6B</t>
+  </si>
+  <si>
+    <t>55v4Tv</t>
+  </si>
+  <si>
+    <t>1dreZD</t>
+  </si>
+  <si>
+    <t>69hr2D</t>
+  </si>
+  <si>
+    <t>MSKqJt</t>
+  </si>
+  <si>
+    <t>fti86U</t>
+  </si>
+  <si>
+    <t>vQ4TQT</t>
+  </si>
+  <si>
+    <t>Rb8opD</t>
+  </si>
+  <si>
+    <t>NqR3Dv</t>
+  </si>
+  <si>
+    <t>gbsdJr</t>
+  </si>
+  <si>
+    <t>uwDlxU</t>
+  </si>
+  <si>
+    <t>126KZr</t>
+  </si>
+  <si>
+    <t>vDzXoO</t>
+  </si>
+  <si>
+    <t>lzt6IM</t>
+  </si>
+  <si>
+    <t>igbAZZ</t>
+  </si>
+  <si>
+    <t>CIT9we</t>
+  </si>
+  <si>
+    <t>AnUbwR</t>
+  </si>
+  <si>
+    <t>GRbFgK</t>
+  </si>
+  <si>
+    <t>UYXbdo</t>
+  </si>
+  <si>
+    <t>YZjYlf</t>
+  </si>
+  <si>
+    <t>lzyxuO</t>
+  </si>
+  <si>
+    <t>fsfPyt</t>
+  </si>
+  <si>
+    <t>oEnpld</t>
+  </si>
+  <si>
+    <t>qlfLh5</t>
+  </si>
+  <si>
+    <t>cLiP0u</t>
+  </si>
+  <si>
+    <t>cId6aS</t>
+  </si>
+  <si>
+    <t>MWzMBF</t>
+  </si>
+  <si>
+    <t>rrhtmZ</t>
+  </si>
+  <si>
+    <t>VZm4m9</t>
+  </si>
+  <si>
+    <t>s4YJ4n</t>
+  </si>
+  <si>
+    <t>OadmSl</t>
+  </si>
+  <si>
+    <t>13PmPW</t>
+  </si>
+  <si>
+    <t>fH4v0C</t>
+  </si>
+  <si>
+    <t>gUyiYG</t>
+  </si>
+  <si>
+    <t>APpEBq</t>
+  </si>
+  <si>
+    <t>bD9Z2L</t>
+  </si>
+  <si>
+    <t>iMSes6</t>
+  </si>
+  <si>
+    <t>odDFYM</t>
+  </si>
+  <si>
+    <t>nmqCpM</t>
+  </si>
+  <si>
+    <t>feVloc</t>
+  </si>
+  <si>
+    <t>mfrSuz</t>
+  </si>
+  <si>
+    <t>WA4woq</t>
+  </si>
+  <si>
+    <t>8jyvNc</t>
+  </si>
+  <si>
+    <t>SMzJQn</t>
+  </si>
+  <si>
+    <t>l1wiAw</t>
+  </si>
+  <si>
+    <t>PblgV4</t>
+  </si>
+  <si>
+    <t>orOlky</t>
+  </si>
+  <si>
+    <t>005qEA</t>
+  </si>
+  <si>
+    <t>FkLOiT</t>
+  </si>
+  <si>
+    <t>xHQjoa</t>
+  </si>
+  <si>
+    <t>MDN7WG</t>
+  </si>
+  <si>
+    <t>uGkFP3</t>
+  </si>
+  <si>
+    <t>mcCItp</t>
+  </si>
+  <si>
+    <t>0AsSDk</t>
+  </si>
+  <si>
+    <t>va1IVi</t>
+  </si>
+  <si>
+    <t>DRZX0p</t>
+  </si>
+  <si>
+    <t>0VMAIw</t>
+  </si>
+  <si>
+    <t>QP7IMk</t>
+  </si>
+  <si>
+    <t>rxitqv</t>
   </si>
 </sst>
 </file>
@@ -606,7 +822,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Finalização do BDD todos os testes
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/HUB_Appium/TestData/BancoDados.xlsx
+++ b/src/main/java/br/com/rsinet/HUB_Appium/TestData/BancoDados.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="133">
   <si>
     <t>Trocar@123</t>
   </si>
@@ -416,6 +416,21 @@
   </si>
   <si>
     <t>Cn8o34</t>
+  </si>
+  <si>
+    <t>KqqQa4</t>
+  </si>
+  <si>
+    <t>VlmFkE</t>
+  </si>
+  <si>
+    <t>Kjhhna</t>
+  </si>
+  <si>
+    <t>c2LYoG</t>
+  </si>
+  <si>
+    <t>UWsvDH</t>
   </si>
 </sst>
 </file>
@@ -882,7 +897,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>

</xml_diff>